<commit_message>
Clothing features based on old clothing trained model added. Corresponding Correlation Data updated as well. Note the ImageFeatures clothing values aren't final.
</commit_message>
<xml_diff>
--- a/Data/ImagesFeatures/aranyajohar.xlsx
+++ b/Data/ImagesFeatures/aranyajohar.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -430,7 +430,11 @@
       <c r="F2" t="n">
         <v>30.135</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Jodhpurs,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -459,7 +463,11 @@
       <c r="F3" t="n">
         <v>31.055</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Parka,Gauchos</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,7 +496,11 @@
       <c r="F4" t="n">
         <v>30.135</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Jodhpurs</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -517,7 +529,11 @@
       <c r="F5" t="n">
         <v>23.776</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -546,7 +562,11 @@
       <c r="F6" t="n">
         <v>26.396</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Blouse,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -575,7 +595,11 @@
       <c r="F7" t="n">
         <v>29.517</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -604,7 +628,11 @@
       <c r="F8" t="n">
         <v>30.135</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Blouse,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -633,7 +661,11 @@
       <c r="F9" t="n">
         <v>26.558</v>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -662,7 +694,11 @@
       <c r="F10" t="n">
         <v>34.726</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -691,7 +727,11 @@
       <c r="F11" t="n">
         <v>24.512</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Kaftan,Tee</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -720,7 +760,11 @@
       <c r="F12" t="n">
         <v>30.135</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -749,7 +793,11 @@
       <c r="F13" t="n">
         <v>30.135</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Parka,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -778,7 +826,11 @@
       <c r="F14" t="n">
         <v>36.468</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -807,7 +859,11 @@
       <c r="F15" t="n">
         <v>25.589</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Trunks,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -836,7 +892,11 @@
       <c r="F16" t="n">
         <v>30.135</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Blouse,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -865,7 +925,11 @@
       <c r="F17" t="n">
         <v>30.135</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Blouse,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -894,7 +958,11 @@
       <c r="F18" t="n">
         <v>26.685</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -923,7 +991,11 @@
       <c r="F19" t="n">
         <v>29.607</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -952,7 +1024,11 @@
       <c r="F20" t="n">
         <v>31.113</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Blouse,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -981,7 +1057,11 @@
       <c r="F21" t="n">
         <v>30.135</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Trunks,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1010,7 +1090,11 @@
       <c r="F22" t="n">
         <v>22.316</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Kaftan,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1039,7 +1123,11 @@
       <c r="F23" t="n">
         <v>25.784</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1068,7 +1156,11 @@
       <c r="F24" t="n">
         <v>29.676</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Blouse,Caftan</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1097,7 +1189,11 @@
       <c r="F25" t="n">
         <v>30.135</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Trunks,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1126,7 +1222,11 @@
       <c r="F26" t="n">
         <v>24.746</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1155,7 +1255,11 @@
       <c r="F27" t="n">
         <v>26.413</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Halter,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1184,7 +1288,11 @@
       <c r="F28" t="n">
         <v>30.135</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Blazer,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1213,7 +1321,11 @@
       <c r="F29" t="n">
         <v>30.135</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1242,7 +1354,11 @@
       <c r="F30" t="n">
         <v>29.046</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1271,7 +1387,11 @@
       <c r="F31" t="n">
         <v>46.69</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1300,7 +1420,11 @@
       <c r="F32" t="n">
         <v>28.915</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1329,7 +1453,11 @@
       <c r="F33" t="n">
         <v>29.449</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1358,7 +1486,11 @@
       <c r="F34" t="n">
         <v>30.671</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Halter,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1387,7 +1519,11 @@
       <c r="F35" t="n">
         <v>26.974</v>
       </c>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1416,7 +1552,11 @@
       <c r="F36" t="n">
         <v>30.135</v>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1445,7 +1585,11 @@
       <c r="F37" t="n">
         <v>29.981</v>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1474,7 +1618,11 @@
       <c r="F38" t="n">
         <v>28.555</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Halter,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1503,7 +1651,11 @@
       <c r="F39" t="n">
         <v>30.135</v>
       </c>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Parka,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1532,7 +1684,11 @@
       <c r="F40" t="n">
         <v>35.799</v>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1561,7 +1717,11 @@
       <c r="F41" t="n">
         <v>29.069</v>
       </c>
-      <c r="G41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Parka,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1590,7 +1750,11 @@
       <c r="F42" t="n">
         <v>25.037</v>
       </c>
-      <c r="G42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Dress,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1619,7 +1783,11 @@
       <c r="F43" t="n">
         <v>30.988</v>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1648,7 +1816,11 @@
       <c r="F44" t="n">
         <v>32.732</v>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Sweatpants,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1677,7 +1849,11 @@
       <c r="F45" t="n">
         <v>33.059</v>
       </c>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Turtleneck,Top</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1706,7 +1882,11 @@
       <c r="F46" t="n">
         <v>30.135</v>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1735,7 +1915,11 @@
       <c r="F47" t="n">
         <v>30.135</v>
       </c>
-      <c r="G47" t="inlineStr"/>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1764,7 +1948,11 @@
       <c r="F48" t="n">
         <v>30.135</v>
       </c>
-      <c r="G48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1793,7 +1981,11 @@
       <c r="F49" t="n">
         <v>33.874</v>
       </c>
-      <c r="G49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1822,7 +2014,11 @@
       <c r="F50" t="n">
         <v>31.581</v>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1851,7 +2047,11 @@
       <c r="F51" t="n">
         <v>30.135</v>
       </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Jodhpurs,Parka</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1880,7 +2080,11 @@
       <c r="F52" t="n">
         <v>30.296</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1909,7 +2113,11 @@
       <c r="F53" t="n">
         <v>30.135</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Tee,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1938,7 +2146,11 @@
       <c r="F54" t="n">
         <v>26.51</v>
       </c>
-      <c r="G54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Caftan,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1967,7 +2179,11 @@
       <c r="F55" t="n">
         <v>25.787</v>
       </c>
-      <c r="G55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Parka,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1996,7 +2212,11 @@
       <c r="F56" t="n">
         <v>29.304</v>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Cutoffs</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2025,7 +2245,11 @@
       <c r="F57" t="n">
         <v>28.817</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Parka</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2054,7 +2278,11 @@
       <c r="F58" t="n">
         <v>35.271</v>
       </c>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2083,7 +2311,11 @@
       <c r="F59" t="n">
         <v>34.613</v>
       </c>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2112,7 +2344,11 @@
       <c r="F60" t="n">
         <v>29.002</v>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Trunks,Sweatpants</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2141,7 +2377,11 @@
       <c r="F61" t="n">
         <v>27.403</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Caftan,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2170,7 +2410,11 @@
       <c r="F62" t="n">
         <v>25.163</v>
       </c>
-      <c r="G62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Parka,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2199,7 +2443,11 @@
       <c r="F63" t="n">
         <v>34.173</v>
       </c>
-      <c r="G63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Blazer,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2228,7 +2476,11 @@
       <c r="F64" t="n">
         <v>30.135</v>
       </c>
-      <c r="G64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2257,7 +2509,11 @@
       <c r="F65" t="n">
         <v>30.135</v>
       </c>
-      <c r="G65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2286,7 +2542,11 @@
       <c r="F66" t="n">
         <v>34.923</v>
       </c>
-      <c r="G66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2315,7 +2575,11 @@
       <c r="F67" t="n">
         <v>38.894</v>
       </c>
-      <c r="G67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Caftan,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2344,7 +2608,11 @@
       <c r="F68" t="n">
         <v>30.135</v>
       </c>
-      <c r="G68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Gauchos,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2373,7 +2641,11 @@
       <c r="F69" t="n">
         <v>29.572</v>
       </c>
-      <c r="G69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Blouse,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2402,7 +2674,11 @@
       <c r="F70" t="n">
         <v>30.791</v>
       </c>
-      <c r="G70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Kaftan,Parka</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2431,7 +2707,11 @@
       <c r="F71" t="n">
         <v>34.025</v>
       </c>
-      <c r="G71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2460,7 +2740,11 @@
       <c r="F72" t="n">
         <v>26.123</v>
       </c>
-      <c r="G72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Trunks,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2489,7 +2773,11 @@
       <c r="F73" t="n">
         <v>40.459</v>
       </c>
-      <c r="G73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Halter,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2518,7 +2806,11 @@
       <c r="F74" t="n">
         <v>30.135</v>
       </c>
-      <c r="G74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2547,7 +2839,11 @@
       <c r="F75" t="n">
         <v>35.443</v>
       </c>
-      <c r="G75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2576,7 +2872,11 @@
       <c r="F76" t="n">
         <v>30.135</v>
       </c>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Kaftan,Tee</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2605,7 +2905,11 @@
       <c r="F77" t="n">
         <v>30.038</v>
       </c>
-      <c r="G77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Kaftan,Dress</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2634,7 +2938,11 @@
       <c r="F78" t="n">
         <v>25.354</v>
       </c>
-      <c r="G78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Tee</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2663,7 +2971,11 @@
       <c r="F79" t="n">
         <v>37.263</v>
       </c>
-      <c r="G79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2692,7 +3004,11 @@
       <c r="F80" t="n">
         <v>30.805</v>
       </c>
-      <c r="G80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2721,7 +3037,11 @@
       <c r="F81" t="n">
         <v>31.36</v>
       </c>
-      <c r="G81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Caftan,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2750,7 +3070,11 @@
       <c r="F82" t="n">
         <v>27.783</v>
       </c>
-      <c r="G82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Turtleneck,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2779,7 +3103,11 @@
       <c r="F83" t="n">
         <v>37.352</v>
       </c>
-      <c r="G83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Turtleneck,Jodhpurs</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2808,7 +3136,11 @@
       <c r="F84" t="n">
         <v>30.804</v>
       </c>
-      <c r="G84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Blouse,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2837,7 +3169,11 @@
       <c r="F85" t="n">
         <v>30.135</v>
       </c>
-      <c r="G85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Trunks,Caftan</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2866,7 +3202,11 @@
       <c r="F86" t="n">
         <v>36.761</v>
       </c>
-      <c r="G86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Trunks,Caftan</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2895,7 +3235,11 @@
       <c r="F87" t="n">
         <v>30.135</v>
       </c>
-      <c r="G87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Turtleneck,Blazer</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2924,7 +3268,11 @@
       <c r="F88" t="n">
         <v>31.829</v>
       </c>
-      <c r="G88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Parka,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2953,7 +3301,11 @@
       <c r="F89" t="n">
         <v>27.537</v>
       </c>
-      <c r="G89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Parka,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2982,7 +3334,11 @@
       <c r="F90" t="n">
         <v>30.135</v>
       </c>
-      <c r="G90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Dress,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3011,7 +3367,11 @@
       <c r="F91" t="n">
         <v>27.02</v>
       </c>
-      <c r="G91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3040,7 +3400,11 @@
       <c r="F92" t="n">
         <v>26.782</v>
       </c>
-      <c r="G92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Caftan</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3069,7 +3433,11 @@
       <c r="F93" t="n">
         <v>30.135</v>
       </c>
-      <c r="G93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Parka,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3098,7 +3466,11 @@
       <c r="F94" t="n">
         <v>23.483</v>
       </c>
-      <c r="G94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Jeggings,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3127,7 +3499,11 @@
       <c r="F95" t="n">
         <v>30.289</v>
       </c>
-      <c r="G95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Blouse,Parka</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3156,7 +3532,11 @@
       <c r="F96" t="n">
         <v>30.135</v>
       </c>
-      <c r="G96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Parka,Gauchos</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3185,7 +3565,11 @@
       <c r="F97" t="n">
         <v>28.735</v>
       </c>
-      <c r="G97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3214,7 +3598,11 @@
       <c r="F98" t="n">
         <v>24.143</v>
       </c>
-      <c r="G98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Blouse,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3243,7 +3631,11 @@
       <c r="F99" t="n">
         <v>27.346</v>
       </c>
-      <c r="G99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Caftan,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3272,7 +3664,11 @@
       <c r="F100" t="n">
         <v>31.131</v>
       </c>
-      <c r="G100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3301,7 +3697,11 @@
       <c r="F101" t="n">
         <v>27.963</v>
       </c>
-      <c r="G101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Trunks,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3330,7 +3730,11 @@
       <c r="F102" t="n">
         <v>30.135</v>
       </c>
-      <c r="G102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Dress,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3359,7 +3763,11 @@
       <c r="F103" t="n">
         <v>30.046</v>
       </c>
-      <c r="G103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Blouse,Jumpsuit</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3388,7 +3796,11 @@
       <c r="F104" t="n">
         <v>31.883</v>
       </c>
-      <c r="G104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3417,7 +3829,11 @@
       <c r="F105" t="n">
         <v>25.014</v>
       </c>
-      <c r="G105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Halter,Blouse</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3446,7 +3862,11 @@
       <c r="F106" t="n">
         <v>28.029</v>
       </c>
-      <c r="G106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Caftan,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3475,7 +3895,11 @@
       <c r="F107" t="n">
         <v>30.135</v>
       </c>
-      <c r="G107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Caftan,Parka</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3504,7 +3928,11 @@
       <c r="F108" t="n">
         <v>28.428</v>
       </c>
-      <c r="G108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Halter</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3533,7 +3961,11 @@
       <c r="F109" t="n">
         <v>33.638</v>
       </c>
-      <c r="G109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3562,7 +3994,11 @@
       <c r="F110" t="n">
         <v>35.921</v>
       </c>
-      <c r="G110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Halter,Kaftan</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3591,7 +4027,11 @@
       <c r="F111" t="n">
         <v>30.135</v>
       </c>
-      <c r="G111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Dress,Trunks</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3620,9 +4060,13 @@
       <c r="F112" t="n">
         <v>30.135</v>
       </c>
-      <c r="G112" t="inlineStr"/>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Jumpsuit,Tee</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>